<commit_message>
Auf jährliche Nachfrage umgestiegen
</commit_message>
<xml_diff>
--- a/Data/sensitivity-analysis.xlsx
+++ b/Data/sensitivity-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annel\Documents\Locating-APLs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFFF75-5625-4876-B78B-6F0A41544B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B582DFF0-0EAC-4FDF-9251-C882EF4D750A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{BB1C52BF-C5D3-4F86-A824-41C71A320735}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
-  <si>
-    <t>DHL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>Heuristik</t>
   </si>
@@ -98,9 +95,6 @@
     <t>Number of opened APLs</t>
   </si>
   <si>
-    <t>237,967m</t>
-  </si>
-  <si>
     <t>Mean Reliability</t>
   </si>
   <si>
@@ -240,6 +234,9 @@
   </si>
   <si>
     <t>Infeasible</t>
+  </si>
+  <si>
+    <t>216,376m</t>
   </si>
 </sst>
 </file>
@@ -297,7 +294,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,14 +320,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -339,14 +335,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -359,18 +365,18 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -458,8 +464,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FE849FE-0F20-457D-91F8-537ED9744974}" name="Tabelle1" displayName="Tabelle1" ref="A1:Q16" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:Q16" xr:uid="{9FE849FE-0F20-457D-91F8-537ED9744974}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FE849FE-0F20-457D-91F8-537ED9744974}" name="Tabelle1" displayName="Tabelle1" ref="A1:Q15" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:Q15" xr:uid="{9FE849FE-0F20-457D-91F8-537ED9744974}"/>
   <tableColumns count="17">
     <tableColumn id="15" xr3:uid="{E897A7E3-BAEB-4C16-A342-C76F6747445C}" name="Test Case" dataDxfId="9"/>
     <tableColumn id="1" xr3:uid="{666BA25E-2C0C-435E-ABC5-DFFC2868B108}" name="Parameter" dataDxfId="8"/>
@@ -476,8 +482,8 @@
     <tableColumn id="11" xr3:uid="{71BA0B31-675C-480E-B687-AFAFE32D091E}" name="Total setup costs" dataDxfId="4"/>
     <tableColumn id="10" xr3:uid="{1EDC6398-4D87-4FBA-851B-6BAA603FD5A5}" name="Mean Reliability" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{A0EA4B7D-3D44-4ADB-966A-6910F1B3B2F4}" name="Avg. daily delivery route " dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{B0E6C52F-0911-4BA8-9DD1-A650904603A4}" name="Combined costs" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{E6E3F93D-4CE0-4715-B581-9216A1EDC3AD}" name="Remark" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{B0E6C52F-0911-4BA8-9DD1-A650904603A4}" name="Combined costs" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{E6E3F93D-4CE0-4715-B581-9216A1EDC3AD}" name="Remark" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -780,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C0388D-1D83-4A59-ACFE-6176EA6FCED9}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,75 +812,75 @@
   <sheetData>
     <row r="1" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>4000</v>
@@ -882,48 +888,47 @@
       <c r="H2">
         <v>15</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>250</v>
       </c>
-      <c r="J2" s="4">
-        <v>39</v>
-      </c>
-      <c r="K2" s="4">
+      <c r="J2">
+        <v>38</v>
+      </c>
+      <c r="K2">
         <v>10</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="M2" s="9">
-        <v>214500</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0.84719999999999995</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="4"/>
+      <c r="M2" s="8">
+        <v>209000</v>
+      </c>
+      <c r="N2">
+        <v>0.82210000000000005</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>4000</v>
@@ -931,90 +936,90 @@
       <c r="H3">
         <v>15</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>250</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="12">
         <v>64</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="12">
         <v>10</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="12">
         <v>12</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="13">
         <v>352000</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="12">
         <v>0.99150000000000005</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="12">
+        <v>60</v>
+      </c>
+      <c r="K4" s="12">
+        <v>10</v>
+      </c>
+      <c r="L4" s="12">
+        <v>12</v>
+      </c>
+      <c r="M4" s="13">
+        <v>330000</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.9919</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>15</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="4">
-        <v>60</v>
-      </c>
-      <c r="K4" s="4">
-        <v>10</v>
-      </c>
-      <c r="L4" s="4">
-        <v>12</v>
-      </c>
-      <c r="M4" s="9">
-        <v>330000</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.9919</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>4000</v>
@@ -1022,48 +1027,47 @@
       <c r="H5">
         <v>15</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>250</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="12">
         <v>36</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="12">
         <v>10</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="12">
         <v>5</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="13">
         <v>198000</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="12">
         <v>0.67589999999999995</v>
       </c>
-      <c r="O5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="4"/>
+      <c r="O5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>6</v>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>4000</v>
@@ -1071,50 +1075,50 @@
       <c r="H6">
         <v>15</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>250</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="12">
         <v>35</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="12">
         <v>10</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="12">
         <v>5</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="13">
         <v>192500</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="12">
         <v>0.72670000000000001</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="4" t="s">
-        <v>47</v>
+      <c r="O6" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>5</v>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>4000</v>
@@ -1122,99 +1126,98 @@
       <c r="H7">
         <v>15</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>250</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="12">
         <v>38</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="12">
         <v>10</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="12">
         <v>5</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="13">
         <v>209000</v>
       </c>
       <c r="N7" s="12">
         <v>0.77500000000000002</v>
       </c>
-      <c r="O7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="4"/>
+      <c r="O7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>5</v>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>4000</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>16</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>250</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="12">
         <v>38</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="12">
         <v>10</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="12">
         <v>4</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="13">
         <v>209000</v>
       </c>
       <c r="N8" s="12">
         <v>0.93740000000000001</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="9"/>
+      <c r="Q8" t="s">
         <v>49</v>
-      </c>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
+      <c r="B9" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>4000</v>
@@ -1222,50 +1225,50 @@
       <c r="H9">
         <v>15</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>250</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="12">
         <v>35</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="15">
         <v>2</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="12">
         <v>1</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="13">
         <v>192500</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="12">
         <v>0.83699999999999997</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="9"/>
+      <c r="Q9" t="s">
         <v>52</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="4" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>4000</v>
@@ -1273,50 +1276,50 @@
       <c r="H10">
         <v>15</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>250</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="12">
         <v>41</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="15">
         <v>25</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="12">
         <v>4</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="13">
         <v>225500</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="12">
         <v>0.84309999999999996</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="9"/>
+      <c r="Q10" t="s">
         <v>55</v>
-      </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>10</v>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="3">
         <v>3000</v>
@@ -1324,50 +1327,50 @@
       <c r="H11">
         <v>15</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>250</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="12">
         <v>49</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="12">
         <v>10</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="12">
         <v>3</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="13">
         <v>269500</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="12">
         <v>0.80259999999999998</v>
       </c>
-      <c r="O11" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="4" t="s">
-        <v>59</v>
+      <c r="O11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="P11" s="9"/>
+      <c r="Q11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>9</v>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3">
         <v>5000</v>
@@ -1375,50 +1378,50 @@
       <c r="H12">
         <v>15</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <v>300</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="12">
         <v>33</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="12">
         <v>10</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="12">
         <v>5</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="13">
         <v>181500</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="12">
         <v>0.90069999999999995</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="O12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" t="s">
         <v>63</v>
       </c>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="4" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>4000</v>
@@ -1426,48 +1429,47 @@
       <c r="H13">
         <v>15</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>200</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="12">
         <v>39</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="12">
         <v>10</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="12">
         <v>5</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="13">
         <v>214500</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="12">
         <v>0.84719999999999995</v>
       </c>
-      <c r="O13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="4"/>
+      <c r="O13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>13</v>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>4000</v>
@@ -1475,48 +1477,47 @@
       <c r="H14">
         <v>15</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>300</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="12">
         <v>39</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="12">
         <v>10</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="12">
         <v>5</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="13">
         <v>214500</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="12">
         <v>0.84719999999999995</v>
       </c>
-      <c r="O14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="4"/>
+      <c r="O14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>4000</v>
@@ -1524,96 +1525,46 @@
       <c r="H15">
         <v>15</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>250</v>
       </c>
-      <c r="J15" s="4">
-        <v>39</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="15">
-        <v>214500</v>
-      </c>
-      <c r="N15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <v>4000</v>
-      </c>
-      <c r="H16">
-        <v>15</v>
-      </c>
-      <c r="I16" s="7">
-        <v>250</v>
-      </c>
-      <c r="J16" s="10">
+      <c r="J15" s="17">
         <v>40</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="15">
+      <c r="K15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="18">
         <v>220000</v>
       </c>
-      <c r="N16" s="10">
-        <v>0.8044</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="4"/>
+      <c r="N15" s="17">
+        <v>0.80559999999999998</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.35">
-      <c r="F19" t="s">
+      <c r="N19" t="s">
         <v>62</v>
-      </c>
-      <c r="J19" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="6:14" x14ac:dyDescent="0.35">
-      <c r="N20" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>